<commit_message>
new feature: support multiple commands per line (currently NOT for multiline tests!)
</commit_message>
<xml_diff>
--- a/core/src/test/resources/loader-test.xlsx
+++ b/core/src/test/resources/loader-test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\development\workspace\jexunit\core\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB068DC-3F88-4E27-B478-944917CF87A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7257C12-5A17-4A55-BFF6-601911A23BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{59860967-8268-434C-8853-F4CC7A473CD1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
   <si>
     <t>COMMAND</t>
   </si>
@@ -58,6 +58,18 @@
   </si>
   <si>
     <t>val4</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -416,15 +428,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ECFE3D6-A52B-4E8A-828A-0941A992B87C}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -440,8 +452,32 @@
       <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -457,8 +493,32 @@
       <c r="E2">
         <v>1</v>
       </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -474,8 +534,32 @@
       <c r="E3">
         <v>0</v>
       </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>13</v>
+      </c>
+      <c r="J3">
+        <v>27</v>
+      </c>
+      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -490,6 +574,21 @@
       </c>
       <c r="E4">
         <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>20</v>
+      </c>
+      <c r="I4">
+        <v>30</v>
+      </c>
+      <c r="J4">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>